<commit_message>
chages in fakha excel sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Hello</t>
   </si>
   <si>
     <t xml:space="preserve">Dude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mister</t>
   </si>
   <si>
     <t xml:space="preserve">fruits</t>
@@ -190,15 +193,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,6 +211,9 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -215,6 +221,9 @@
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -241,38 +250,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -282,7 +291,7 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -292,7 +301,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -302,7 +311,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -312,7 +321,7 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -322,7 +331,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>

<commit_message>
create insertion query from sheet must give value types
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,15 +21,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">Hello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mister</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+  <si>
+    <t xml:space="preserve">dobpaymentrequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creationdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifieddate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creationinfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modificationinfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentstates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paymentType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purchaseUnitId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paymentForm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'2019000001'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'2018-08-05 09:02:00'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Amira.Atya'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'["Draft"]'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'GENERAL'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'CASH’</t>
   </si>
   <si>
     <t xml:space="preserve">fruits</t>
@@ -193,43 +238,107 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -242,46 +351,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I65536"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="13.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -291,7 +400,7 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -301,7 +410,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -311,7 +420,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -321,7 +430,7 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -331,7 +440,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -350,7 +459,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
used factory pattern to implement different kinds of queries
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="payment-request" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t xml:space="preserve">dobpaymentrequest</t>
   </si>
@@ -74,7 +74,19 @@
     <t xml:space="preserve">'GENERAL'</t>
   </si>
   <si>
-    <t xml:space="preserve">'CASH’</t>
+    <t xml:space="preserve">'CASH'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float</t>
   </si>
   <si>
     <t xml:space="preserve">fruits</t>
@@ -238,10 +250,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -333,6 +345,41 @@
       </c>
       <c r="K3" s="0" t="n">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -366,31 +413,31 @@
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -400,7 +447,7 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -410,7 +457,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -420,7 +467,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -430,7 +477,7 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -440,7 +487,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>

<commit_message>
create SheetQueryForm to take sheet name and form list of queries for whole sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -21,9 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="36">
   <si>
     <t xml:space="preserve">dobpaymentrequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insertion</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -250,10 +253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,40 +279,43 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,31 +323,31 @@
         <v>1001</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>20</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>1000</v>
@@ -349,37 +355,263 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="K8" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="J9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="B14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>21</v>
+      <c r="J14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -413,31 +645,31 @@
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -447,7 +679,7 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -457,7 +689,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -467,7 +699,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -477,7 +709,7 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -487,7 +719,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>

<commit_message>
completed TDD cycle for query creator from excel sheets
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -8,8 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="payment-request" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="testSheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,14 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">insert</t>
+  </si>
   <si>
     <t xml:space="preserve">dobpaymentrequest</t>
   </si>
   <si>
-    <t xml:space="preserve">insertion</t>
-  </si>
-  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -92,43 +91,10 @@
     <t xml:space="preserve">Float</t>
   </si>
   <si>
-    <t xml:space="preserve">fruits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price per kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buying amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sellin amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">profit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sel per day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">profit per day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mango</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teen shoki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3enab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kiwi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cantaloupe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bateekh</t>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'’</t>
   </si>
 </sst>
 </file>
@@ -138,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -161,32 +127,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Open_sansregular"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,16 +170,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,13 +199,13 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
@@ -279,7 +222,7 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -462,8 +405,8 @@
       <c r="J8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="0" t="n">
-        <v>1000</v>
+      <c r="K8" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +516,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>1000</v>
@@ -623,125 +566,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I1048576"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="13.89"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="2"/>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
completed TDD cycles for All payment request create story queries
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="testSheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="paymentRequest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="33">
   <si>
     <t xml:space="preserve">insert</t>
   </si>
@@ -95,6 +96,30 @@
   </si>
   <si>
     <t xml:space="preserve">'’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EntityUserCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'DObPaymentRequest'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alter-sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dobpaymentrequest_id_seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence-restart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'2019000004'</t>
   </si>
 </sst>
 </file>
@@ -196,16 +221,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
@@ -557,6 +582,60 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -566,4 +645,240 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.39"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change row number after forming query inside query creator
</commit_message>
<xml_diff>
--- a/src/main/resources/Fakha.xlsx
+++ b/src/main/resources/Fakha.xlsx
@@ -129,7 +129,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -151,6 +151,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,12 +203,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,22 +233,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.53"/>
@@ -287,37 +299,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="I3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -400,37 +412,37 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="I8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -513,37 +525,37 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J13" s="0" t="s">
+      <c r="I13" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -590,49 +602,49 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>1005</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -654,7 +666,7 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -662,14 +674,14 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.39"/>
   </cols>
   <sheetData>

</xml_diff>